<commit_message>
Update criteria with Talc criterion
</commit_message>
<xml_diff>
--- a/master_list.xlsx
+++ b/master_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelmelnick/Work/repos/hyperspectral_notebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88354C2F-E960-0942-A98F-83E247F49FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB1B99B-288B-2641-9606-7358D69E597F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="23260" windowHeight="14160" xr2:uid="{9070629F-1B76-40C5-A6EC-E70AAA098343}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>Product ID</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t>F-900</t>
+  </si>
+  <si>
+    <t>F-2080</t>
+  </si>
+  <si>
+    <t>talc</t>
   </si>
 </sst>
 </file>
@@ -618,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CEAED50-895A-4027-8BBE-28EFAF12A6BD}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -870,16 +876,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C16" s="5">
-        <v>2145</v>
+        <v>2070</v>
       </c>
       <c r="D16" s="5">
-        <v>2185</v>
+        <v>2100</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>10</v>
@@ -887,16 +893,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="5">
+        <v>2145</v>
+      </c>
+      <c r="D17" s="5">
         <v>2185</v>
-      </c>
-      <c r="D17" s="5">
-        <v>2230</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>10</v>
@@ -904,16 +910,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="5">
+        <v>2185</v>
+      </c>
+      <c r="D18" s="5">
         <v>2230</v>
-      </c>
-      <c r="D18" s="5">
-        <v>2265</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>10</v>
@@ -921,16 +927,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="5">
-        <v>2220</v>
+        <v>2230</v>
       </c>
       <c r="D19" s="5">
-        <v>2300</v>
+        <v>2265</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>10</v>
@@ -938,16 +944,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="5">
-        <v>2270</v>
+        <v>2220</v>
       </c>
       <c r="D20" s="5">
-        <v>2330</v>
+        <v>2300</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>10</v>
@@ -955,16 +961,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C21" s="5">
-        <v>2325</v>
+        <v>2270</v>
       </c>
       <c r="D21" s="5">
-        <v>2370</v>
+        <v>2330</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>10</v>
@@ -972,16 +978,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C22" s="5">
-        <v>2345</v>
+        <v>2325</v>
       </c>
       <c r="D22" s="5">
-        <v>2390</v>
+        <v>2370</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>10</v>
@@ -989,23 +995,40 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="5">
+        <v>2345</v>
+      </c>
+      <c r="D23" s="5">
+        <v>2390</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B24" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C24" s="5">
         <v>2375</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D24" s="5">
         <v>2415</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
+      <c r="E24" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>